<commit_message>
fix export excel 1
</commit_message>
<xml_diff>
--- a/outputExcel/KPI.xlsx
+++ b/outputExcel/KPI.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nhanvienL1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nhanvienL2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nhanvienL3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nhanvienNoLevel" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nhanvienSVCNTS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Nhóm L1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Nhóm L2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Nhóm L3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Nhóm SVCNTS" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,105 +444,100 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>employeeId</t>
+          <t>fullName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>fullName</t>
+          <t>level</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>level</t>
+          <t>teamName</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>teamId</t>
+          <t>Loại</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>teamName</t>
+          <t>krId</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Loại</t>
+          <t>KR phòng</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>KR phòng</t>
+          <t>KR team</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>KR team</t>
+          <t>KR cá nhân</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>KR cá nhân</t>
+          <t>Công thức tính</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Công thức tính</t>
+          <t>Nguồn dữ liệu</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Nguồn dữ liệu</t>
+          <t>Định kỳ tính</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Định kỳ tính</t>
+          <t>Đơn vị tính</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Đơn vị tính</t>
+          <t>Điều kiện</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Điều kiện</t>
+          <t>Norm</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Norm</t>
+          <t>% Trọng số chỉ tiêu</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>% Trọng số chỉ tiêu</t>
+          <t>Kết quả</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Kết quả</t>
+          <t>Tỷ lệ</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Tỷ lệ</t>
+          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
+          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -551,97 +545,94 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Giang Pham</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PHG</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>BE</t>
-        </is>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>KPI</t>
+          <t>tét2321</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Đảm bảo tiến độ và chất lượng nghiên cứu công nghệ mới áp dụng vào các dự án</t>
+          <t>tét2321</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Đảm bảo tiến độ và chất lượng nghiên cứu công nghệ mới generative AI áp dụng vào các dự án</t>
+          <t>tét2321</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Đảm bảo hoàn thành 100% tiến độ áp dụng Chatbot, generative AI vào dự án Storybook/Low code được CBQL confirm </t>
+          <t>Báo cáo được CBQL confirm</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Báo cáo được CBQL confirm</t>
+          <t>email</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Mail</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>NUM</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>EQUAL</t>
         </is>
       </c>
       <c r="O2" t="n">
         <v>100</v>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
-      <c r="Q2" t="n">
-        <v>80</v>
+      <c r="P2" t="n">
+        <v>78</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
           <t>No data</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>No data</t>
-        </is>
+      <c r="S2" t="n">
+        <v>168</v>
       </c>
       <c r="T2" t="n">
         <v>168</v>
       </c>
-      <c r="U2" t="n">
-        <v>168</v>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>No data</t>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>dfqwq</t>
         </is>
       </c>
     </row>
@@ -656,7 +647,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -672,109 +663,727 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>employeeId</t>
+          <t>fullName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>fullName</t>
+          <t>level</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>level</t>
+          <t>teamName</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>teamId</t>
+          <t>Loại</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>teamName</t>
+          <t>krId</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Loại</t>
+          <t>KR phòng</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>KR phòng</t>
+          <t>KR team</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>KR team</t>
+          <t>KR cá nhân</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>KR cá nhân</t>
+          <t>Công thức tính</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Công thức tính</t>
+          <t>Nguồn dữ liệu</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Nguồn dữ liệu</t>
+          <t>Định kỳ tính</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Định kỳ tính</t>
+          <t>Đơn vị tính</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Đơn vị tính</t>
+          <t>Điều kiện</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Điều kiện</t>
+          <t>Norm</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Norm</t>
+          <t>% Trọng số chỉ tiêu</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>% Trọng số chỉ tiêu</t>
+          <t>Kết quả</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Kết quả</t>
+          <t>Tỷ lệ</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Tỷ lệ</t>
+          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
+          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
           <t>Note</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Phung Hoang</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Đảm bảo tiến độ và chất lượng nghiên cứu công nghệ mới áp dụng vào các dự án</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Đảm bảo tiến độ và chất lượng nghiên cứu công nghệ mới generative AI áp dụng vào các dự án</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Đảm bảo hoàn thành 100% tiến độ áp dụng Chatbot, generative AI vào dự án Storybook/Low code được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>100</v>
+      </c>
+      <c r="P2" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>168</v>
+      </c>
+      <c r="T2" t="n">
+        <v>168</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Phung Hoang</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Đảm bảo tiến độ và chất lượng nghiên cứu công nghệ mới áp dụng vào các dự án</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Đảm bảo tiến độ và chất lượng nghiên cứu công nghệ mới generative AI áp dụng vào các dự án</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Đảm bảo hoàn thành 100% tiến độ áp dụng Chatbot, generative AI vào dự án Storybook/Low code được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>100</v>
+      </c>
+      <c r="P3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>168</v>
+      </c>
+      <c r="T3" t="n">
+        <v>168</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Phung Hoang</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Đảm bảo tiến độ và chất lượng nghiên cứu công nghệ mới áp dụng vào các dự án</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Đảm bảo tiến độ và chất lượng nghiên cứu công nghệ mới generative AI áp dụng vào các dự án</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Đảm bảo hoàn thành 100% tiến độ áp dụng Chatbot, generative AI vào dự án Storybook/Low code được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>100</v>
+      </c>
+      <c r="P4" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>168</v>
+      </c>
+      <c r="T4" t="n">
+        <v>168</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Phung Hoang</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>100</v>
+      </c>
+      <c r="P5" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>168</v>
+      </c>
+      <c r="T5" t="n">
+        <v>168</v>
+      </c>
+      <c r="U5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Phung Hoang</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>100</v>
+      </c>
+      <c r="P6" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>168</v>
+      </c>
+      <c r="T6" t="n">
+        <v>168</v>
+      </c>
+      <c r="U6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Phung Hoang</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>100</v>
+      </c>
+      <c r="P7" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>168</v>
+      </c>
+      <c r="T7" t="n">
+        <v>168</v>
+      </c>
+      <c r="U7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Phung Hoang</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>test kpi 3 1</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>100</v>
+      </c>
+      <c r="P8" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>168</v>
+      </c>
+      <c r="T8" t="n">
+        <v>168</v>
+      </c>
+      <c r="U8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -787,7 +1396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -803,109 +1412,282 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>employeeId</t>
+          <t>fullName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>fullName</t>
+          <t>level</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>level</t>
+          <t>teamName</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>teamId</t>
+          <t>Loại</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>teamName</t>
+          <t>krId</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Loại</t>
+          <t>KR phòng</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>KR phòng</t>
+          <t>KR team</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>KR team</t>
+          <t>KR cá nhân</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>KR cá nhân</t>
+          <t>Công thức tính</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Công thức tính</t>
+          <t>Nguồn dữ liệu</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Nguồn dữ liệu</t>
+          <t>Định kỳ tính</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Định kỳ tính</t>
+          <t>Đơn vị tính</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Đơn vị tính</t>
+          <t>Điều kiện</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Điều kiện</t>
+          <t>Norm</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Norm</t>
+          <t>% Trọng số chỉ tiêu</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>% Trọng số chỉ tiêu</t>
+          <t>Kết quả</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Kết quả</t>
+          <t>Tỷ lệ</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Tỷ lệ</t>
+          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
+          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
           <t>Note</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>pham</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>test kpi 4 1</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>test kpi 4 1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>test kpi 4 1</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>100</v>
+      </c>
+      <c r="P2" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>168</v>
+      </c>
+      <c r="T2" t="n">
+        <v>168</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>pham</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>KPI</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>test kpi 4 1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>test kpi 4 1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>test kpi 4 1</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>100</v>
+      </c>
+      <c r="P3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>168</v>
+      </c>
+      <c r="T3" t="n">
+        <v>168</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -918,7 +1700,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -934,236 +1716,100 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>employeeId</t>
+          <t>fullName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>fullName</t>
+          <t>level</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>level</t>
+          <t>teamName</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>teamId</t>
+          <t>Loại</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>teamName</t>
+          <t>krId</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Loại</t>
+          <t>KR phòng</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>KR phòng</t>
+          <t>KR team</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>KR team</t>
+          <t>KR cá nhân</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>KR cá nhân</t>
+          <t>Công thức tính</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Công thức tính</t>
+          <t>Nguồn dữ liệu</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Nguồn dữ liệu</t>
+          <t>Định kỳ tính</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Định kỳ tính</t>
+          <t>Đơn vị tính</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Đơn vị tính</t>
+          <t>Điều kiện</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Điều kiện</t>
+          <t>Norm</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Norm</t>
+          <t>% Trọng số chỉ tiêu</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>% Trọng số chỉ tiêu</t>
+          <t>Kết quả</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Kết quả</t>
+          <t>Tỷ lệ</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Tỷ lệ</t>
+          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
+          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>employeeId</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>fullName</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>teamId</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>teamName</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Loại</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>KR phòng</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>KR team</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>KR cá nhân</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Công thức tính</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Nguồn dữ liệu</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Định kỳ tính</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Đơn vị tính</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Điều kiện</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Norm</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>% Trọng số chỉ tiêu</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Kết quả</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Tỷ lệ</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Note</t>
         </is>

</xml_diff>